<commit_message>
Added 3 types of lighting, models, and textures
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -911,7 +911,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="H4" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1051,11 +1051,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1071,11 +1071,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1112,7 +1116,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1180,11 +1184,11 @@
       </c>
       <c r="H8" s="10">
         <f>H4+IF(H4 &lt; 22, IF(K4+H4 &gt; 22, 22- H4, K4),0)</f>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
@@ -1245,7 +1249,7 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
@@ -1400,11 +1404,15 @@
       <c r="D18" s="5">
         <v>3</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1662,11 +1670,15 @@
       <c r="D30" s="5">
         <v>3</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G30" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1687,11 +1699,15 @@
       <c r="D31" s="5">
         <v>3</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1712,11 +1728,15 @@
       <c r="D32" s="5">
         <v>3</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G32" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1737,11 +1757,15 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>

</xml_diff>

<commit_message>
added skybox and multithreading
</commit_message>
<xml_diff>
--- a/Graphics II Project Rubric.xlsx
+++ b/Graphics II Project Rubric.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>http://www.opengl-tutorial.org/beginners-tutorials/tutorial-7-model-loading/</t>
   </si>
 </sst>
 </file>
@@ -913,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -1046,7 +1049,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1054,11 +1057,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1119,7 +1122,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1197,7 +1200,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1254,11 +1257,11 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -1538,11 +1541,15 @@
       <c r="D23" s="5">
         <v>4</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1763,14 +1770,14 @@
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2240,11 +2247,15 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="E55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2265,11 +2276,15 @@
       <c r="D56" s="5">
         <v>5</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G56" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2974,7 +2989,9 @@
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
+      <c r="A95" s="16" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="16"/>
@@ -3064,7 +3081,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>